<commit_message>
added more tests and included more columns
</commit_message>
<xml_diff>
--- a/LogisticalRegressionColumns.xlsx
+++ b/LogisticalRegressionColumns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\stats-for-ai-final-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE3E36D-DFDF-4635-B82B-4D9B9C199A8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3EF847-B8C6-4B5A-984E-ED75BC92C71C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="1710" windowWidth="29040" windowHeight="15720" xr2:uid="{945B195D-1B2A-4A7C-929B-ACBFE41A23A2}"/>
   </bookViews>
@@ -197,10 +197,10 @@
     <t>Binary if we remove enrolled</t>
   </si>
   <si>
-    <t>Not Yet</t>
-  </si>
-  <si>
     <t>Might be ordinal but can treat as continuous for this probably</t>
+  </si>
+  <si>
+    <t>Yes?</t>
   </si>
 </sst>
 </file>
@@ -244,9 +244,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,7 +565,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -610,7 +611,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
         <v>48</v>
@@ -665,7 +666,7 @@
       <c r="B7" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D7" t="s">
@@ -679,7 +680,7 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D8" t="s">
@@ -693,8 +694,8 @@
       <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="C9" t="s">
-        <v>43</v>
+      <c r="C9" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D9" t="s">
         <v>48</v>
@@ -707,8 +708,8 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" t="s">
-        <v>43</v>
+      <c r="C10" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D10" t="s">
         <v>48</v>
@@ -721,8 +722,8 @@
       <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="C11" t="s">
-        <v>43</v>
+      <c r="C11" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D11" t="s">
         <v>48</v>
@@ -735,8 +736,8 @@
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="C12" t="s">
-        <v>43</v>
+      <c r="C12" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D12" t="s">
         <v>48</v>
@@ -749,8 +750,8 @@
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="C13" t="s">
-        <v>43</v>
+      <c r="C13" s="2" t="s">
+        <v>54</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
@@ -865,7 +866,7 @@
         <v>39</v>
       </c>
       <c r="D21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
@@ -890,7 +891,7 @@
         <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
         <v>51</v>
@@ -904,7 +905,7 @@
         <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
         <v>51</v>
@@ -918,7 +919,7 @@
         <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
         <v>51</v>
@@ -932,7 +933,7 @@
         <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
         <v>51</v>
@@ -946,7 +947,7 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
         <v>51</v>
@@ -960,7 +961,7 @@
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D28" t="s">
         <v>51</v>
@@ -974,7 +975,7 @@
         <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D29" t="s">
         <v>51</v>
@@ -988,7 +989,7 @@
         <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s">
         <v>51</v>
@@ -1002,7 +1003,7 @@
         <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D31" t="s">
         <v>51</v>
@@ -1016,7 +1017,7 @@
         <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D32" t="s">
         <v>51</v>
@@ -1030,7 +1031,7 @@
         <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
         <v>51</v>
@@ -1044,7 +1045,7 @@
         <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D34" t="s">
         <v>51</v>

</xml_diff>